<commit_message>
A modified file is changed
</commit_message>
<xml_diff>
--- a/Тест-кейс Steam11.xlsx
+++ b/Тест-кейс Steam11.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiril\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiril\Desktop\projects Skillfactory\KirTsy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E58254-6DD6-4415-A199-A7273B1B97F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA31CA89-E396-4139-B558-6713AB7ABBD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="49">
   <si>
     <t>Тест Кейс №/ID</t>
   </si>
@@ -170,6 +170,9 @@
   </si>
   <si>
     <t>Загрузилась страница с необходимыми результатами.</t>
+  </si>
+  <si>
+    <t>fgfgfgf</t>
   </si>
 </sst>
 </file>
@@ -9678,7 +9681,7 @@
   <dimension ref="A1:C999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -9705,7 +9708,9 @@
       <c r="B2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="6" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">

</xml_diff>